<commit_message>
fix PMID nan error
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/ReferenceSummary_Mar25.xlsx
+++ b/Pubmed/CCHF/ReferenceSummary_Mar25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/Library/CloudStorage/Dropbox/Shared/___SystematicReviewsAI/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3EEDDC-D9F3-B941-832D-47FB3118FC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE2A43A-0ABA-3543-924B-5CF9496D7BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="500" windowWidth="24220" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21580" yWindow="500" windowWidth="27160" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3620,14 +3620,6 @@
   </si>
   <si>
     <t>AY905625
-AF481802
-AJ010648
-AJ010649
-AY049082
-AY277672
-AY366375
-AY366376
-AY366378
 AY905626
 AY905627
 AY905628
@@ -3666,28 +3658,11 @@
 AY905661
 AY905662
 AY905663
-M25150
-M86624
-U04958
-U15020
-U15021
-U15022
-U15023
-U15024
-U15089
-U15090
-U15091
-U15092
-U15093
 U84635
 U84636
 U84637
 U84638
-U84639
-U88412
-U88413
-U88414
-U88415</t>
+U84639</t>
   </si>
 </sst>
 </file>
@@ -4247,9 +4222,9 @@
   </sheetPr>
   <dimension ref="A1:AU182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W11" sqref="W11"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="125" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R187" sqref="R187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>